<commit_message>
Alterada a logo, e desocultada planilha de aco bruto
</commit_message>
<xml_diff>
--- a/padrao/quantitativoPadrao.xlsx
+++ b/padrao/quantitativoPadrao.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gusta\source\repos\quantitativosExtraidosTQS\padrao\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gusta\source\repos\QuantTqs\padrao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E9DF96B-7A79-4C9D-9935-0283776F6071}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AD9DF2E-0756-4C80-AFA2-F593513668EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{FB9F9397-F0D6-405E-BB1F-A3B5E634906A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{FB9F9397-F0D6-405E-BB1F-A3B5E634906A}"/>
   </bookViews>
   <sheets>
     <sheet name="Resumo" sheetId="1" r:id="rId1"/>
-    <sheet name="Descritivo" sheetId="2" r:id="rId2"/>
-    <sheet name="Aco_Pranchado" sheetId="4" r:id="rId3"/>
-    <sheet name="Aco_Pranchado_bruto" sheetId="3" state="hidden" r:id="rId4"/>
+    <sheet name="Aco_Pranchado" sheetId="4" r:id="rId2"/>
+    <sheet name="Descritivo_Concreto" sheetId="2" r:id="rId3"/>
+    <sheet name="Aco_Pranchado_bruto" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -785,14 +785,14 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1133,26 +1133,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C593AAD4-62CE-463C-B622-67DAFD987A8C}">
   <dimension ref="A1:M27"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" topLeftCell="A2" zoomScale="85" zoomScaleNormal="100" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" zoomScale="85" zoomScaleNormal="100" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.33203125" customWidth="1"/>
-    <col min="2" max="4" width="10.44140625" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" customWidth="1"/>
-    <col min="6" max="7" width="10.44140625" customWidth="1"/>
+    <col min="1" max="1" width="20.28515625" customWidth="1"/>
+    <col min="2" max="4" width="10.42578125" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" customWidth="1"/>
+    <col min="6" max="7" width="10.42578125" customWidth="1"/>
     <col min="8" max="8" width="15" customWidth="1"/>
-    <col min="9" max="9" width="10.44140625" customWidth="1"/>
+    <col min="9" max="9" width="10.42578125" customWidth="1"/>
     <col min="10" max="10" width="12" customWidth="1"/>
-    <col min="11" max="11" width="10.6640625" customWidth="1"/>
-    <col min="12" max="12" width="10.44140625" customWidth="1"/>
-    <col min="13" max="13" width="8.88671875" customWidth="1"/>
-    <col min="14" max="16384" width="8.88671875" hidden="1"/>
+    <col min="11" max="11" width="10.7109375" customWidth="1"/>
+    <col min="12" max="12" width="10.42578125" customWidth="1"/>
+    <col min="13" max="13" width="8.85546875" customWidth="1"/>
+    <col min="14" max="16384" width="8.85546875" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="44" t="s">
         <v>63</v>
       </c>
@@ -1168,7 +1168,7 @@
       <c r="K1" s="44"/>
       <c r="L1" s="44"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>28</v>
       </c>
@@ -1184,7 +1184,7 @@
       <c r="K2" s="3"/>
       <c r="L2" s="4"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>29</v>
       </c>
@@ -1200,7 +1200,7 @@
       <c r="K3" s="3"/>
       <c r="L3" s="4"/>
     </row>
-    <row r="4" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="40" t="s">
         <v>0</v>
       </c>
@@ -1238,7 +1238,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="8"/>
       <c r="B5" s="9" t="s">
         <v>5</v>
@@ -1274,7 +1274,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="8"/>
       <c r="B6" s="9"/>
       <c r="C6" s="9"/>
@@ -1288,7 +1288,7 @@
       <c r="K6" s="10"/>
       <c r="L6" s="11"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="33" t="s">
         <v>44</v>
       </c>
@@ -1337,7 +1337,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="13"/>
       <c r="B8" s="13"/>
       <c r="C8" s="13"/>
@@ -1351,7 +1351,7 @@
       <c r="K8" s="13"/>
       <c r="L8" s="13"/>
     </row>
-    <row r="9" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" ht="18" x14ac:dyDescent="0.25">
       <c r="A9" s="14"/>
       <c r="B9" s="15" t="s">
         <v>8</v>
@@ -1375,7 +1375,7 @@
       <c r="K9" s="13"/>
       <c r="L9" s="13"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="14"/>
       <c r="B10" s="17" t="s">
         <v>13</v>
@@ -1399,7 +1399,7 @@
       <c r="K10" s="13"/>
       <c r="L10" s="13"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="37" t="s">
         <v>18</v>
       </c>
@@ -1430,7 +1430,7 @@
       <c r="K11" s="13"/>
       <c r="L11" s="13"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="19"/>
       <c r="B12" s="19"/>
       <c r="C12" s="19"/>
@@ -1444,7 +1444,7 @@
       <c r="K12" s="13"/>
       <c r="L12" s="13"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="19" t="s">
         <v>19</v>
       </c>
@@ -1460,7 +1460,7 @@
       <c r="K13" s="13"/>
       <c r="L13" s="13"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="19" t="s">
         <v>20</v>
       </c>
@@ -1476,7 +1476,7 @@
       <c r="K14" s="13"/>
       <c r="L14" s="13"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="19" t="s">
         <v>21</v>
       </c>
@@ -1492,7 +1492,7 @@
       <c r="K15" s="13"/>
       <c r="L15" s="13"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="19" t="s">
         <v>22</v>
       </c>
@@ -1508,7 +1508,7 @@
       <c r="K16" s="13"/>
       <c r="L16" s="13"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
         <v>43</v>
       </c>
@@ -1524,7 +1524,7 @@
       <c r="K17" s="13"/>
       <c r="L17" s="13"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="19" t="s">
         <v>23</v>
       </c>
@@ -1540,57 +1540,57 @@
       <c r="K18" s="13"/>
       <c r="L18" s="13"/>
     </row>
-    <row r="20" spans="1:12" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="21" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
-      <c r="F21" s="46" t="s">
+    <row r="20" spans="1:12" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="F21" s="45" t="s">
         <v>47</v>
       </c>
-      <c r="G21" s="46"/>
+      <c r="G21" s="45"/>
       <c r="H21" s="27">
         <v>2.7</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="34.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F22" s="47" t="s">
+    <row r="22" spans="1:12" ht="34.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F22" s="46" t="s">
         <v>50</v>
       </c>
-      <c r="G22" s="47"/>
+      <c r="G22" s="46"/>
       <c r="H22" s="26">
         <v>105</v>
       </c>
-      <c r="I22" s="47" t="s">
+      <c r="I22" s="46" t="s">
         <v>51</v>
       </c>
-      <c r="J22" s="47"/>
-      <c r="K22" s="47"/>
+      <c r="J22" s="46"/>
+      <c r="K22" s="46"/>
       <c r="L22" s="26">
         <v>2.5</v>
       </c>
     </row>
-    <row r="23" spans="1:12" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="24" spans="1:12" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="25" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:12" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="45" t="s">
+    <row r="27" spans="1:12" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="47" t="s">
         <v>49</v>
       </c>
-      <c r="B27" s="45"/>
-      <c r="C27" s="45"/>
-      <c r="D27" s="45"/>
-      <c r="E27" s="45"/>
-      <c r="F27" s="45"/>
-      <c r="G27" s="45"/>
-      <c r="H27" s="45"/>
-      <c r="I27" s="45"/>
+      <c r="B27" s="47"/>
+      <c r="C27" s="47"/>
+      <c r="D27" s="47"/>
+      <c r="E27" s="47"/>
+      <c r="F27" s="47"/>
+      <c r="G27" s="47"/>
+      <c r="H27" s="47"/>
+      <c r="I27" s="47"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1612,25 +1612,95 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{611AC2FB-9DCD-4BD4-8149-751888AC5A12}">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="37.140625" customWidth="1"/>
+    <col min="2" max="3" width="12.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="51" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="51"/>
+      <c r="C1" s="52"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="7"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="4"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="40" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" s="41" t="s">
+        <v>60</v>
+      </c>
+      <c r="C4" s="42" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="28"/>
+      <c r="B5" s="31"/>
+      <c r="C5" s="32"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="29"/>
+      <c r="B6" s="30"/>
+      <c r="C6" s="43"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" s="34"/>
+      <c r="C7" s="35"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C8218E8-19D1-406A-A3F8-24EB4FB87F13}">
   <dimension ref="A1:P3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H15" sqref="H15"/>
+      <selection pane="bottomLeft" activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="12.109375" customWidth="1"/>
-    <col min="5" max="5" width="13.109375" customWidth="1"/>
-    <col min="6" max="6" width="15.6640625" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" customWidth="1"/>
     <col min="8" max="11" width="11" customWidth="1"/>
-    <col min="12" max="12" width="11.109375" customWidth="1"/>
-    <col min="13" max="16" width="12.6640625" customWidth="1"/>
+    <col min="12" max="12" width="11.140625" customWidth="1"/>
+    <col min="13" max="16" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="48" t="s">
         <v>39</v>
       </c>
@@ -1652,7 +1722,7 @@
       <c r="O1" s="49"/>
       <c r="P1" s="50"/>
     </row>
-    <row r="2" spans="1:16" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" ht="57.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="40" t="s">
         <v>32</v>
       </c>
@@ -1696,7 +1766,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="8"/>
       <c r="B3" s="10" t="s">
         <v>7</v>
@@ -1744,91 +1814,21 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{611AC2FB-9DCD-4BD4-8149-751888AC5A12}">
-  <dimension ref="A1:C7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="37.109375" customWidth="1"/>
-    <col min="2" max="3" width="12.6640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="51" t="s">
-        <v>61</v>
-      </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="52"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C2" s="7"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="4"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="40" t="s">
-        <v>53</v>
-      </c>
-      <c r="B4" s="41" t="s">
-        <v>60</v>
-      </c>
-      <c r="C4" s="42" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="28"/>
-      <c r="B5" s="31"/>
-      <c r="C5" s="32"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="29"/>
-      <c r="B6" s="30"/>
-      <c r="C6" s="43"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="33" t="s">
-        <v>44</v>
-      </c>
-      <c r="B7" s="34"/>
-      <c r="C7" s="35"/>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:C1"/>
-  </mergeCells>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E091A5E-78D4-4718-960B-336A63B7AB12}">
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="A1:E1048576"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.109375" customWidth="1"/>
-    <col min="2" max="5" width="12.6640625" customWidth="1"/>
+    <col min="1" max="1" width="37.140625" customWidth="1"/>
+    <col min="2" max="5" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="51" t="s">
         <v>52</v>
       </c>
@@ -1837,7 +1837,7 @@
       <c r="D1" s="51"/>
       <c r="E1" s="52"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>28</v>
       </c>
@@ -1846,7 +1846,7 @@
       <c r="D2" s="3"/>
       <c r="E2" s="4"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>29</v>
       </c>
@@ -1855,7 +1855,7 @@
       <c r="D3" s="3"/>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>53</v>
       </c>
@@ -1872,7 +1872,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="8"/>
       <c r="B5" s="9"/>
       <c r="C5" s="9" t="s">
@@ -1885,14 +1885,14 @@
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="8"/>
       <c r="B6" s="9"/>
       <c r="C6" s="9"/>
       <c r="D6" s="10"/>
       <c r="E6" s="11"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>44</v>
       </c>

</xml_diff>